<commit_message>
Savepoint; Account separation (exlusion by process) implemented; still some work remaining although tests show successful; upgraded the request update function to cancel orders open at broker if in [queued|pending] state to reduce order module overhead involved w/ the cancel/resubmit broker limitation; next up: new tests to complete fcrt;
</commit_message>
<xml_diff>
--- a/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
+++ b/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15638" tabRatio="1000"/>
+    <workbookView windowHeight="15638" tabRatio="1000" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="request" sheetId="2" r:id="rId1"/>
-    <sheet name="orders" sheetId="1" r:id="rId2"/>
-    <sheet name="vw_requests" sheetId="7" r:id="rId3"/>
-    <sheet name="vw_orders" sheetId="6" r:id="rId4"/>
-    <sheet name="vw_api_requests" sheetId="11" r:id="rId5"/>
+    <sheet name="Summary" sheetId="12" r:id="rId1"/>
+    <sheet name="request" sheetId="2" r:id="rId2"/>
+    <sheet name="orders" sheetId="1" r:id="rId3"/>
+    <sheet name="vw_requests" sheetId="7" r:id="rId4"/>
+    <sheet name="vw_orders" sheetId="6" r:id="rId5"/>
+    <sheet name="vw_api_requests" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="baseline">request!$A$3:$A$22</definedName>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="60">
   <si>
     <t>REQUEST</t>
   </si>
@@ -77,7 +78,7 @@
     <t>update_time</t>
   </si>
   <si>
-    <t>ORDER</t>
+    <t>ORDERS</t>
   </si>
   <si>
     <t>order_id</t>
@@ -207,15 +208,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="178" formatCode="m/d/yy\ h:mm\.ss.000"/>
+  <numFmts count="7">
+    <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm\.ss.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -234,6 +234,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -243,7 +265,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,9 +309,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,30 +363,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -309,74 +377,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -387,25 +387,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,157 +567,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,6 +578,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -606,6 +615,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -622,26 +646,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,17 +670,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -683,148 +683,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -832,37 +832,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1184,9 +1184,73 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="5" width="18.3407407407407" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="10" t="str">
+        <f>request!A1</f>
+        <v>REQUEST</v>
+      </c>
+      <c r="B1" s="10" t="str">
+        <f>orders!A1</f>
+        <v>ORDERS</v>
+      </c>
+      <c r="C1" s="10" t="str">
+        <f>vw_requests!A1</f>
+        <v>VW_REQUESTS</v>
+      </c>
+      <c r="D1" s="10" t="str">
+        <f>vw_orders!A1</f>
+        <v>VW_ORDERS</v>
+      </c>
+      <c r="E1" s="10" t="str">
+        <f>vw_api_requests!A1</f>
+        <v>VW_API_REQUESTS</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="11">
+        <f>COUNTA(request!A3:A1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="11">
+        <f>COUNTA(orders!A3:A1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="11">
+        <f>COUNTA(vw_requests!A3:A1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="11">
+        <f>COUNTA(vw_orders!A3:A1048576)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="11">
+        <f>COUNTA(vw_api_requests!A3:A1048576)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1215,10 +1279,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <f>COUNTA(A3:A1048576)</f>
-        <v>0</v>
-      </c>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="2" t="s">
@@ -1270,121 +1331,6 @@
         <v>16</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:U2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
-  <cols>
-    <col min="1" max="1" width="15.0444444444444" customWidth="1"/>
-    <col min="2" max="2" width="15.3851851851852" style="8" customWidth="1"/>
-    <col min="3" max="3" width="9.39259259259259" customWidth="1"/>
-    <col min="4" max="4" width="8.39259259259259" customWidth="1"/>
-    <col min="5" max="5" width="13.562962962963" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.57037037037037" customWidth="1"/>
-    <col min="7" max="7" width="6.87407407407407" customWidth="1"/>
-    <col min="8" max="8" width="13.8518518518519" customWidth="1"/>
-    <col min="9" max="9" width="10.0592592592593" customWidth="1"/>
-    <col min="10" max="10" width="13.8444444444444" customWidth="1"/>
-    <col min="11" max="11" width="14.2518518518519" customWidth="1"/>
-    <col min="12" max="12" width="12.0740740740741" style="9" customWidth="1"/>
-    <col min="13" max="13" width="9.17037037037037" customWidth="1"/>
-    <col min="14" max="14" width="12.5925925925926" customWidth="1"/>
-    <col min="15" max="15" width="13.6888888888889" customWidth="1"/>
-    <col min="16" max="16" width="14.1481481481481" style="9" customWidth="1"/>
-    <col min="17" max="17" width="15.4592592592593" style="9" customWidth="1"/>
-    <col min="18" max="18" width="12.162962962963" customWidth="1"/>
-    <col min="19" max="19" width="9.77037037037037" customWidth="1"/>
-    <col min="20" max="21" width="19.2666666666667" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="10">
-        <f>COUNTA(A3:A1048576)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="U2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1397,18 +1343,130 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="15.0444444444444" customWidth="1"/>
+    <col min="2" max="2" width="15.3851851851852" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.39259259259259" customWidth="1"/>
+    <col min="4" max="4" width="8.39259259259259" customWidth="1"/>
+    <col min="5" max="5" width="13.562962962963" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.57037037037037" customWidth="1"/>
+    <col min="7" max="7" width="6.87407407407407" customWidth="1"/>
+    <col min="8" max="8" width="13.8518518518519" customWidth="1"/>
+    <col min="9" max="9" width="10.0592592592593" customWidth="1"/>
+    <col min="10" max="10" width="13.8444444444444" customWidth="1"/>
+    <col min="11" max="11" width="14.2518518518519" customWidth="1"/>
+    <col min="12" max="12" width="12.0740740740741" style="8" customWidth="1"/>
+    <col min="13" max="13" width="9.17037037037037" customWidth="1"/>
+    <col min="14" max="14" width="12.5925925925926" customWidth="1"/>
+    <col min="15" max="15" width="13.6888888888889" customWidth="1"/>
+    <col min="16" max="16" width="14.1481481481481" style="8" customWidth="1"/>
+    <col min="17" max="17" width="15.4592592592593" style="8" customWidth="1"/>
+    <col min="18" max="18" width="12.162962962963" customWidth="1"/>
+    <col min="19" max="19" width="9.77037037037037" customWidth="1"/>
+    <col min="20" max="21" width="19.2666666666667" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="15.0444444444444" customWidth="1"/>
-    <col min="2" max="2" width="15.3851851851852" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.3851851851852" style="3" customWidth="1"/>
     <col min="3" max="3" width="8.37037037037037" customWidth="1"/>
     <col min="4" max="4" width="11.5703703703704" customWidth="1"/>
     <col min="5" max="5" width="13.162962962963" customWidth="1"/>
@@ -1435,10 +1493,7 @@
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="6">
-        <f>COUNTA(A3:A1048576)</f>
-        <v>0</v>
-      </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" s="2" t="s">
@@ -1517,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:AU2"/>
@@ -1525,18 +1580,18 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="15.0444444444444" customWidth="1"/>
-    <col min="2" max="2" width="15.3851851851852" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.3851851851852" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.0444444444444" customWidth="1"/>
     <col min="4" max="4" width="8.37037037037037" customWidth="1"/>
     <col min="5" max="5" width="11.5703703703704" customWidth="1"/>
     <col min="6" max="6" width="13.162962962963" customWidth="1"/>
-    <col min="7" max="7" width="14.6592592592593" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.6592592592593" style="4" customWidth="1"/>
     <col min="8" max="8" width="13.162962962963" customWidth="1"/>
     <col min="9" max="9" width="15.5555555555556" customWidth="1"/>
     <col min="10" max="10" width="14.1555555555556" customWidth="1"/>
@@ -1581,10 +1636,7 @@
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6">
-        <f>COUNTA(A3:A1048576)</f>
-        <v>0</v>
-      </c>
+      <c r="B1" s="5"/>
     </row>
     <row r="2" spans="1:47">
       <c r="A2" s="2" t="s">
@@ -1605,7 +1657,7 @@
       <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1735,82 +1787,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A1048524" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="P1048570" sqref="P1048570"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="7.48888888888889" customWidth="1"/>
-    <col min="2" max="2" width="13.162962962963" customWidth="1"/>
-    <col min="3" max="3" width="12.8518518518519" customWidth="1"/>
-    <col min="4" max="4" width="12.7481481481481" customWidth="1"/>
-    <col min="5" max="5" width="5.08148148148148" customWidth="1"/>
-    <col min="6" max="6" width="10.6666666666667" customWidth="1"/>
-    <col min="7" max="7" width="9.39259259259259" customWidth="1"/>
-    <col min="8" max="8" width="8.39259259259259" customWidth="1"/>
-    <col min="9" max="9" width="11.6592592592593" customWidth="1"/>
-    <col min="10" max="10" width="9.07407407407407" customWidth="1"/>
-    <col min="11" max="11" width="15.0444444444444" customWidth="1"/>
-    <col min="12" max="12" width="51.0962962962963" customWidth="1"/>
-    <col min="13" max="13" width="19.2666666666667" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77037037037037" customWidth="1"/>
+    <col min="2" max="2" width="9.66666666666667" customWidth="1"/>
+    <col min="3" max="3" width="13.162962962963" customWidth="1"/>
+    <col min="4" max="4" width="12.8518518518519" customWidth="1"/>
+    <col min="5" max="5" width="12.7481481481481" customWidth="1"/>
+    <col min="6" max="6" width="5.08148148148148" customWidth="1"/>
+    <col min="7" max="7" width="10.6666666666667" customWidth="1"/>
+    <col min="8" max="8" width="9.39259259259259" customWidth="1"/>
+    <col min="9" max="9" width="8.39259259259259" customWidth="1"/>
+    <col min="10" max="10" width="11.6592592592593" customWidth="1"/>
+    <col min="11" max="11" width="9.07407407407407" customWidth="1"/>
+    <col min="12" max="12" width="15.0444444444444" customWidth="1"/>
+    <col min="13" max="13" width="51.0962962962963" customWidth="1"/>
+    <col min="14" max="14" width="19.7333333333333" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="2">
-        <f>COUNTA(A3:A1048576)</f>
-        <v>0</v>
-      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="N1"/>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Savepoint; fcrt/2.1.1 retest; next up fcrt/2.1.2;
</commit_message>
<xml_diff>
--- a/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
+++ b/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15638" tabRatio="1000" activeTab="5"/>
+    <workbookView windowHeight="15638" tabRatio="1000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -209,13 +209,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm\.ss.000"/>
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm\.ss.000"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -241,13 +241,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -257,31 +250,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -293,6 +265,111 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -300,83 +377,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -387,19 +387,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,13 +519,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,145 +561,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,21 +615,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -640,15 +625,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,6 +644,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -683,148 +683,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -832,31 +832,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1250,7 +1250,7 @@
   <sheetPr/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1792,10 +1792,10 @@
   <sheetPr/>
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A1048524" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="P1048570" sqref="P1048570"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>

</xml_diff>

<commit_message>
Working Release; Many changes to finalize account and schema divsions; FCRT 2.1.1 completed successfuly; this is a working release and est. 75% complete til production ready; next up, stops handling - should go quickly; same methodology as request->orders; finalizing FCRT 2.1.2, 2.1.3 and possibly new FCRT 2.1.4;
</commit_message>
<xml_diff>
--- a/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
+++ b/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15638" tabRatio="508" activeTab="1"/>
+    <workbookView windowHeight="15638" tabRatio="508"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="12" r:id="rId1"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
   <si>
     <t>REQUEST</t>
   </si>
   <si>
     <t>Request</t>
+  </si>
+  <si>
+    <t>Order Id</t>
   </si>
   <si>
     <t>Instrument
@@ -82,7 +85,8 @@
     <t>ORDERS</t>
   </si>
   <si>
-    <t>Order Id</t>
+    <t>Client
+Order Id</t>
   </si>
   <si>
     <t>Order
@@ -119,10 +123,6 @@
   </si>
   <si>
     <t>Account</t>
-  </si>
-  <si>
-    <t>Client
-Order Id</t>
   </si>
   <si>
     <t>instrument
@@ -273,15 +273,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="10">
     <numFmt numFmtId="176" formatCode="0.000000_);[Red]\(0.000000\)"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="177" formatCode="m/d/yy\ h:mm\.ss.000"/>
-    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="179" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm\.ss.000"/>
+    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="182" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -300,8 +300,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,7 +348,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,9 +384,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -338,24 +398,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -368,81 +443,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -453,13 +453,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,169 +621,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -666,21 +666,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -691,21 +676,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,6 +706,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -744,173 +729,188 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -922,7 +922,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -931,22 +931,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1273,8 +1276,8 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1301,19 +1304,19 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="18">
+      <c r="A2" s="19">
         <f>COUNTA(request!A3:A1048575)</f>
         <v>0</v>
       </c>
-      <c r="B2" s="18">
-        <f>COUNTA(orders!A3:A1048576)</f>
+      <c r="B2" s="19">
+        <f>COUNTA(orders!A3:A1048575)</f>
         <v>0</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="19">
         <f>COUNTA(vw_orders!A3:A1048575)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="19">
         <f>COUNTA(vw_api_requests!A3:A1048575)</f>
         <v>0</v>
       </c>
@@ -1327,9 +1330,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1337,39 +1340,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="2" width="16.6444444444444" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.76296296296296" style="1" customWidth="1"/>
-    <col min="5" max="6" width="15.4518518518519" style="14" customWidth="1"/>
-    <col min="7" max="7" width="10.4666666666667" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.4666666666667" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.4666666666667" style="3" customWidth="1"/>
-    <col min="11" max="11" width="74.3777777777778" customWidth="1"/>
-    <col min="12" max="12" width="8.46666666666667" style="10" customWidth="1"/>
-    <col min="13" max="15" width="19.837037037037" style="15" customWidth="1"/>
+    <col min="1" max="3" width="16.6444444444444" style="1" customWidth="1"/>
+    <col min="4" max="5" width="8.76296296296296" style="1" customWidth="1"/>
+    <col min="6" max="7" width="15.4518518518519" style="15" customWidth="1"/>
+    <col min="8" max="8" width="10.4666666666667" style="3" customWidth="1"/>
+    <col min="9" max="10" width="10.4666666666667" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.4666666666667" style="3" customWidth="1"/>
+    <col min="12" max="12" width="74.3777777777778" customWidth="1"/>
+    <col min="13" max="13" width="8.46666666666667" style="10" customWidth="1"/>
+    <col min="14" max="16" width="19.837037037037" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24" customHeight="1" spans="1:10">
+    <row r="1" ht="24" customHeight="1" spans="1:11">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="6"/>
-      <c r="C1"/>
+      <c r="C1" s="6"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
-      <c r="G1" s="10"/>
+      <c r="G1"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
-    <row r="2" ht="40" customHeight="1" spans="1:15">
+    <row r="2" ht="40" customHeight="1" spans="1:16">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
@@ -1384,29 +1388,32 @@
       <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="18" t="s">
         <v>15</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1428,23 +1435,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.0444444444444" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.3851851851852" style="1" customWidth="1"/>
-    <col min="3" max="5" width="13.7481481481481" style="1" customWidth="1"/>
-    <col min="6" max="8" width="15.6518518518519" style="12" customWidth="1"/>
-    <col min="9" max="9" width="12.5925925925926" style="8" customWidth="1"/>
-    <col min="10" max="10" width="13.6888888888889" style="8" customWidth="1"/>
+    <col min="1" max="2" width="15.6518518518519" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.3851851851852" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.7481481481481" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7481481481481" style="12" customWidth="1"/>
+    <col min="7" max="8" width="15.6518518518519" style="12" customWidth="1"/>
+    <col min="9" max="9" width="15.6518518518519" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12.5925925925926" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:10">
       <c r="A1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="B1"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
-      <c r="F1"/>
+      <c r="F1" s="10"/>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
@@ -1452,34 +1460,34 @@
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:10">
       <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1528,7 +1536,7 @@
   <sheetData>
     <row r="1" ht="24" customHeight="1" spans="1:48">
       <c r="A1" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1" s="9"/>
       <c r="D1" s="10"/>
@@ -1577,16 +1585,16 @@
     </row>
     <row r="2" ht="40" customHeight="1" spans="1:48">
       <c r="A2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>29</v>
@@ -1610,7 +1618,7 @@
         <v>35</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>36</v>
@@ -1622,7 +1630,7 @@
         <v>38</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q2" s="11" t="s">
         <v>39</v>
@@ -1631,52 +1639,52 @@
         <v>40</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U2" s="11" t="s">
         <v>41</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Z2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="AA2" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AB2" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AE2" s="7" t="s">
         <v>43</v>
       </c>
       <c r="AF2" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AG2" s="7" t="s">
         <v>44</v>
       </c>
       <c r="AH2" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AI2" s="11" t="s">
         <v>45</v>
@@ -1688,7 +1696,7 @@
         <v>47</v>
       </c>
       <c r="AL2" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AM2" s="11" t="s">
         <v>48</v>
@@ -1709,16 +1717,16 @@
         <v>53</v>
       </c>
       <c r="AS2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AT2" s="11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AU2" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AV2" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="AV2" s="11" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Savepoint; closing in on final solution; launching FCRT tests 2.1, 2.2; next up: leverage management, test findings resolutions, fractal algo integration, then, go live;
</commit_message>
<xml_diff>
--- a/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
+++ b/fcrt/2.1-cli-om/2.1.1-req-no-expiry/Documents/baseline.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>REQUEST</t>
   </si>
@@ -173,6 +173,10 @@
 Type</t>
   </si>
   <si>
+    <t>Auto
+Trade</t>
+  </si>
+  <si>
     <t>Filled
 Size</t>
   </si>
@@ -223,6 +227,9 @@
   </si>
   <si>
     <t>account</t>
+  </si>
+  <si>
+    <t>orderId</t>
   </si>
   <si>
     <t>status</t>
@@ -274,14 +281,14 @@
   <numFmts count="10">
     <numFmt numFmtId="176" formatCode="0.000000_);[Red]\(0.000000\)"/>
     <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="178" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="179" formatCode="m/d/yy\ h:mm\.ss.000"/>
-    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="m/d/yy\ h:mm\.ss.000"/>
+    <numFmt numFmtId="182" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="182" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -300,6 +307,135 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -308,141 +444,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -453,43 +460,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,31 +598,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,67 +616,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,31 +634,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,11 +663,52 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -682,11 +730,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -705,192 +751,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -901,16 +908,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -922,7 +929,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -931,7 +938,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -943,13 +950,13 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1512,9 +1519,10 @@
     <col min="1" max="1" width="11.837037037037" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.2962962962963" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.2962962962963" style="3" customWidth="1"/>
-    <col min="4" max="5" width="16.2962962962963" style="1" customWidth="1"/>
-    <col min="6" max="11" width="11.962962962963" style="1" customWidth="1"/>
-    <col min="12" max="22" width="8.8" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.2962962962963" style="1" customWidth="1"/>
+    <col min="5" max="10" width="11.962962962963" style="1" customWidth="1"/>
+    <col min="11" max="16" width="8.8" style="1" customWidth="1"/>
+    <col min="17" max="22" width="8.79259259259259" style="1" customWidth="1"/>
     <col min="23" max="23" width="15.7111111111111" style="2" customWidth="1"/>
     <col min="24" max="24" width="11.1407407407407" style="2" customWidth="1"/>
     <col min="25" max="25" width="11.1407407407407" style="3" customWidth="1"/>
@@ -1594,61 +1602,61 @@
         <v>2</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="F2" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="G2" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="H2" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="11" t="s">
         <v>35</v>
       </c>
+      <c r="K2" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="L2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="M2" s="11" t="s">
+        <v>37</v>
+      </c>
       <c r="N2" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O2" s="11" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="P2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="11" t="s">
         <v>39</v>
       </c>
+      <c r="Q2" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="R2" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="S2" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="S2" s="11" t="s">
+        <v>9</v>
+      </c>
       <c r="T2" s="11" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="W2" s="7" t="s">
         <v>6</v>
@@ -1660,7 +1668,7 @@
         <v>8</v>
       </c>
       <c r="Z2" s="11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="11" t="s">
         <v>23</v>
@@ -1675,46 +1683,46 @@
         <v>26</v>
       </c>
       <c r="AE2" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="AG2" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AH2" s="11" t="s">
         <v>21</v>
       </c>
       <c r="AI2" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AJ2" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AK2" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AL2" s="11" t="s">
         <v>11</v>
       </c>
       <c r="AM2" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AN2" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AO2" s="11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AP2" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AQ2" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AR2" s="11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AS2" s="7" t="s">
         <v>12</v>
@@ -1738,7 +1746,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -1748,25 +1756,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.79259259259259" defaultRowHeight="14.1" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="7" width="12.3555555555556" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.962962962963" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.39259259259259" style="2" customWidth="1"/>
-    <col min="10" max="10" width="11.6592592592593" style="3" customWidth="1"/>
-    <col min="11" max="11" width="11.8592592592593" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.0444444444444" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.9481481481481" style="1" customWidth="1"/>
-    <col min="14" max="14" width="74.3777777777778" style="4" customWidth="1"/>
-    <col min="15" max="15" width="19.2666666666667" style="5" customWidth="1"/>
+    <col min="1" max="1" width="12.3555555555556" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.9481481481481" style="1" customWidth="1"/>
+    <col min="3" max="8" width="12.3555555555556" style="1" customWidth="1"/>
+    <col min="9" max="10" width="12.6592592592593" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.6592592592593" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.8592592592593" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.0444444444444" style="1" customWidth="1"/>
+    <col min="14" max="14" width="15.9481481481481" style="1" customWidth="1"/>
+    <col min="15" max="15" width="74.3777777777778" style="4" customWidth="1"/>
+    <col min="16" max="16" width="19.2666666666667" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24" customHeight="1" spans="1:15">
+    <row r="1" ht="24" customHeight="1" spans="1:16">
       <c r="A1" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="B1"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1"/>
+      <c r="E1" s="6"/>
       <c r="F1"/>
       <c r="G1"/>
       <c r="H1"/>
@@ -1777,52 +1786,56 @@
       <c r="M1"/>
       <c r="N1"/>
       <c r="O1"/>
+      <c r="P1"/>
     </row>
-    <row r="2" ht="40" customHeight="1" spans="1:15">
+    <row r="2" ht="40" customHeight="1" spans="1:16">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>